<commit_message>
train rcan with histloss
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nnobi\Desktop\FIUBA\Tesis\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C0621B-C92C-4BC8-A667-3A6CC1A9358D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6737C6A-2FBB-4E98-A6B2-8A1269414072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2589" yWindow="3009" windowWidth="16457" windowHeight="9565" xr2:uid="{D9AB7B09-F977-4CED-B019-8CC4CCCC5ABA}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{D9AB7B09-F977-4CED-B019-8CC4CCCC5ABA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Image Super-Resolution Using Deep Convolutional Networks / 1501.00092v3</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>A Review of Image Super-Resolution Approaches Based on Deep Learning and Applications in Remote Sensing</t>
+  </si>
+  <si>
+    <t>The Unreasonable Effectiveness of Deep Features as a Perceptual Metric</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1801.03924?utm_source=chatgpt.com</t>
   </si>
 </sst>
 </file>
@@ -473,19 +479,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6260CA-0A2F-492F-84B0-7083784942F2}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -501,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -509,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -517,7 +523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -525,7 +531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -533,7 +539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -541,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -549,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -557,7 +563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -565,12 +571,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>